<commit_message>
Se suben cambios en los documentos
</commit_message>
<xml_diff>
--- a/extras/docs/R-GC-02 Ficha de metadatos.xlsx
+++ b/extras/docs/R-GC-02 Ficha de metadatos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="9045" tabRatio="500"/>
   </bookViews>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="177">
   <si>
     <t>#</t>
   </si>
@@ -547,12 +542,74 @@
       <t>DEL CONOCIMIENTO</t>
     </r>
   </si>
+  <si>
+    <t>APLICACIÓN WEB PARA EL REGISTRO DE ACTIVIDADES Y PRODUCTOS DE CONFORMIDAD CON EL FORMATO R-DC- 54 DE LAS UNIDADES TECNOLÓGICAS DE SANTANDER</t>
+  </si>
+  <si>
+    <t>Sandy Pauline Cala Sanguino
+Elkin Giovanny Murillo Quintana</t>
+  </si>
+  <si>
+    <t>Roberto Carvajal Salamanca</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Trabajo de Grado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan de Trabajo, Formato R-DC-54, Actividades, Productos, Horarios
+</t>
+  </si>
+  <si>
+    <t>Desarrollo de una aplicación que permite registrar el plan de trabajo de los docentes de las Unidades Tecnológicas de Santander, el software consta de módulos para el registro del horario, actividades y productos del docente, también se incluye un módulo de evaluador y auditor, también se encarga de generar reportes basados en el formato RDC-54 y RDC-26 de la universidad. Se dará a conocer como se estructuro y organizo cada sección del software en cuestión. Además se adiciona algunos problemas que surgieron en el proceso y de las  opciones que se contemplaron para mitigar o solucionar el problema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTA DE FIGURAS .............................................................................................................................. 10
+LISTA DE TABLAS ................................................................................................................................. 10 
+RESUMEN EJECUTIVO.......................................................................................................................  11
+INTRODUCCIÓN...................................................................................................................................  12
+1. DESCRIPCIÓN DEL TRABAJO DE INVESTIGACIÓN ...............................................................  14
+1.1. PLANTEAMIENTO DEL PROBLEMA .......................................................................................... 14
+1.2. JUSTIFICACIÓN.............................................................................................................................  16
+1.3. OBJETIVOS.....................................................................................................................................  17
+1.3.1. OBJETIVO GENERAL................................................................................................................  17
+1.3.2. OBJETIVOS ESPECÍFICOS......................................................................................................  17
+1.4. ESTADO DEL ARTE / ANTECEDENTES...................................................................................  18
+2. MARCOS REFERENCIALES...........................................................................................................  25
+2.1. MARCO TEÓRICO..........................................................................................................................  25
+2.2 MARCO LEGAL................................................................................................................................  27
+2.3 MARCO CONCEPTUAL.................................................................................................................  28
+3. DESARROLLO DEL TRABAJO DE GRADO.................................................................................  30
+3.1. ANALISIS.........................................................................................................................................  30
+3.2 DISEÑO Y ARQUITECTURA.........................................................................................................  34
+3.3 FASE DE DESARROLLO...............................................................................................................  81
+3.4 REVISION Y VERIFICACION.........................................................................................................  93
+4. RESULTADOS...................................................................................................................................  96
+5. CONCLUSIONES..............................................................................................................................  97
+6. RECOMENDACIONES.....................................................................................................................  99
+7. REFERENCIAS BIBLIOGRÁFICAS..............................................................................................  101
+</t>
+  </si>
+  <si>
+    <t>Departamental</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>Documento (.doc)</t>
+  </si>
+  <si>
+    <t>Acceso Abierto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1334,7 +1391,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1574,12 +1631,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1616,6 +1667,12 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1699,6 +1756,78 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="144">
@@ -2297,10 +2426,10 @@
   <dimension ref="B1:AM160"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:T8"/>
+      <selection activeCell="C14" sqref="C14:T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="28.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.625" style="7" customWidth="1"/>
     <col min="2" max="2" width="2.625" style="7" customWidth="1"/>
@@ -2313,7 +2442,7 @@
     <col min="98" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="13.5" customHeight="1">
+    <row r="1" spans="2:39" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -2351,93 +2480,93 @@
       <c r="AK1" s="6"/>
       <c r="AL1" s="6"/>
     </row>
-    <row r="2" spans="2:39" ht="46.5" customHeight="1">
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95" t="s">
+    <row r="2" spans="2:39" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="96" t="s">
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="105" t="s">
         <v>160</v>
       </c>
-      <c r="AD2" s="95"/>
-      <c r="AE2" s="95"/>
-      <c r="AF2" s="95"/>
-      <c r="AG2" s="95"/>
-      <c r="AH2" s="95"/>
-      <c r="AI2" s="95"/>
-      <c r="AJ2" s="95"/>
-      <c r="AK2" s="95"/>
-      <c r="AL2" s="95"/>
-    </row>
-    <row r="3" spans="2:39" ht="28.5" customHeight="1">
-      <c r="C3" s="95" t="s">
+      <c r="AD2" s="104"/>
+      <c r="AE2" s="104"/>
+      <c r="AF2" s="104"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="104"/>
+      <c r="AI2" s="104"/>
+      <c r="AJ2" s="104"/>
+      <c r="AK2" s="104"/>
+      <c r="AL2" s="104"/>
+    </row>
+    <row r="3" spans="2:39" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95" t="s">
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95" t="s">
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+      <c r="AB3" s="104"/>
+      <c r="AC3" s="104" t="s">
         <v>159</v>
       </c>
-      <c r="AD3" s="95"/>
-      <c r="AE3" s="95"/>
-      <c r="AF3" s="95"/>
-      <c r="AG3" s="95"/>
-      <c r="AH3" s="95"/>
-      <c r="AI3" s="95"/>
-      <c r="AJ3" s="95"/>
-      <c r="AK3" s="95"/>
-      <c r="AL3" s="95"/>
-    </row>
-    <row r="4" spans="2:39" ht="15.95" customHeight="1">
+      <c r="AD3" s="104"/>
+      <c r="AE3" s="104"/>
+      <c r="AF3" s="104"/>
+      <c r="AG3" s="104"/>
+      <c r="AH3" s="104"/>
+      <c r="AI3" s="104"/>
+      <c r="AJ3" s="104"/>
+      <c r="AK3" s="104"/>
+      <c r="AL3" s="104"/>
+    </row>
+    <row r="4" spans="2:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="92"/>
       <c r="D4" s="92"/>
       <c r="E4" s="92"/>
@@ -2475,8 +2604,8 @@
       <c r="AK4" s="93"/>
       <c r="AL4" s="93"/>
     </row>
-    <row r="5" spans="2:39" ht="12.95" customHeight="1"/>
-    <row r="6" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="2:39" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2518,7 +2647,7 @@
       <c r="AL6" s="8"/>
       <c r="AM6" s="8"/>
     </row>
-    <row r="7" spans="2:39" ht="11.25" customHeight="1">
+    <row r="7" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="17">
         <v>64</v>
@@ -2570,47 +2699,49 @@
       </c>
       <c r="AM7" s="8"/>
     </row>
-    <row r="8" spans="2:39" ht="53.25" customHeight="1">
+    <row r="8" spans="2:39" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="98"/>
-      <c r="Q8" s="98"/>
-      <c r="R8" s="98"/>
-      <c r="S8" s="98"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="97"/>
-      <c r="V8" s="98"/>
-      <c r="W8" s="98"/>
-      <c r="X8" s="98"/>
-      <c r="Y8" s="98"/>
-      <c r="Z8" s="98"/>
-      <c r="AA8" s="98"/>
-      <c r="AB8" s="98"/>
-      <c r="AC8" s="98"/>
-      <c r="AD8" s="98"/>
-      <c r="AE8" s="98"/>
-      <c r="AF8" s="98"/>
-      <c r="AG8" s="98"/>
-      <c r="AH8" s="98"/>
-      <c r="AI8" s="98"/>
-      <c r="AJ8" s="98"/>
-      <c r="AK8" s="98"/>
-      <c r="AL8" s="99"/>
+      <c r="C8" s="137" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="138"/>
+      <c r="P8" s="138"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="139"/>
+      <c r="U8" s="95"/>
+      <c r="V8" s="96"/>
+      <c r="W8" s="96"/>
+      <c r="X8" s="96"/>
+      <c r="Y8" s="96"/>
+      <c r="Z8" s="96"/>
+      <c r="AA8" s="96"/>
+      <c r="AB8" s="96"/>
+      <c r="AC8" s="96"/>
+      <c r="AD8" s="96"/>
+      <c r="AE8" s="96"/>
+      <c r="AF8" s="96"/>
+      <c r="AG8" s="96"/>
+      <c r="AH8" s="96"/>
+      <c r="AI8" s="96"/>
+      <c r="AJ8" s="96"/>
+      <c r="AK8" s="96"/>
+      <c r="AL8" s="97"/>
       <c r="AM8" s="8"/>
     </row>
-    <row r="9" spans="2:39" ht="12" customHeight="1">
+    <row r="9" spans="2:39" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="17">
         <v>9</v>
@@ -2662,127 +2793,131 @@
       </c>
       <c r="AM9" s="8"/>
     </row>
-    <row r="10" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="101"/>
-      <c r="Q10" s="101"/>
-      <c r="R10" s="101"/>
-      <c r="S10" s="101"/>
-      <c r="T10" s="102"/>
-      <c r="U10" s="100"/>
-      <c r="V10" s="101"/>
-      <c r="W10" s="101"/>
-      <c r="X10" s="101"/>
-      <c r="Y10" s="101"/>
-      <c r="Z10" s="101"/>
-      <c r="AA10" s="101"/>
-      <c r="AB10" s="101"/>
-      <c r="AC10" s="101"/>
-      <c r="AD10" s="101"/>
-      <c r="AE10" s="101"/>
-      <c r="AF10" s="101"/>
-      <c r="AG10" s="101"/>
-      <c r="AH10" s="101"/>
-      <c r="AI10" s="101"/>
-      <c r="AJ10" s="101"/>
-      <c r="AK10" s="101"/>
-      <c r="AL10" s="102"/>
+      <c r="C10" s="141" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="142"/>
+      <c r="S10" s="142"/>
+      <c r="T10" s="143"/>
+      <c r="U10" s="144" t="s">
+        <v>167</v>
+      </c>
+      <c r="V10" s="142"/>
+      <c r="W10" s="142"/>
+      <c r="X10" s="142"/>
+      <c r="Y10" s="142"/>
+      <c r="Z10" s="142"/>
+      <c r="AA10" s="142"/>
+      <c r="AB10" s="142"/>
+      <c r="AC10" s="142"/>
+      <c r="AD10" s="142"/>
+      <c r="AE10" s="142"/>
+      <c r="AF10" s="142"/>
+      <c r="AG10" s="142"/>
+      <c r="AH10" s="142"/>
+      <c r="AI10" s="142"/>
+      <c r="AJ10" s="142"/>
+      <c r="AK10" s="142"/>
+      <c r="AL10" s="143"/>
       <c r="AM10" s="8"/>
     </row>
-    <row r="11" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="101"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="101"/>
-      <c r="R11" s="101"/>
-      <c r="S11" s="101"/>
-      <c r="T11" s="102"/>
-      <c r="U11" s="100"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="101"/>
-      <c r="X11" s="101"/>
-      <c r="Y11" s="101"/>
-      <c r="Z11" s="101"/>
-      <c r="AA11" s="101"/>
-      <c r="AB11" s="101"/>
-      <c r="AC11" s="101"/>
-      <c r="AD11" s="101"/>
-      <c r="AE11" s="101"/>
-      <c r="AF11" s="101"/>
-      <c r="AG11" s="101"/>
-      <c r="AH11" s="101"/>
-      <c r="AI11" s="101"/>
-      <c r="AJ11" s="101"/>
-      <c r="AK11" s="101"/>
-      <c r="AL11" s="102"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="142"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="142"/>
+      <c r="L11" s="142"/>
+      <c r="M11" s="142"/>
+      <c r="N11" s="142"/>
+      <c r="O11" s="142"/>
+      <c r="P11" s="142"/>
+      <c r="Q11" s="142"/>
+      <c r="R11" s="142"/>
+      <c r="S11" s="142"/>
+      <c r="T11" s="143"/>
+      <c r="U11" s="144"/>
+      <c r="V11" s="142"/>
+      <c r="W11" s="142"/>
+      <c r="X11" s="142"/>
+      <c r="Y11" s="142"/>
+      <c r="Z11" s="142"/>
+      <c r="AA11" s="142"/>
+      <c r="AB11" s="142"/>
+      <c r="AC11" s="142"/>
+      <c r="AD11" s="142"/>
+      <c r="AE11" s="142"/>
+      <c r="AF11" s="142"/>
+      <c r="AG11" s="142"/>
+      <c r="AH11" s="142"/>
+      <c r="AI11" s="142"/>
+      <c r="AJ11" s="142"/>
+      <c r="AK11" s="142"/>
+      <c r="AL11" s="143"/>
       <c r="AM11" s="8"/>
     </row>
-    <row r="12" spans="2:39" ht="12.75" customHeight="1">
+    <row r="12" spans="2:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="98"/>
-      <c r="P12" s="98"/>
-      <c r="Q12" s="98"/>
-      <c r="R12" s="98"/>
-      <c r="S12" s="98"/>
-      <c r="T12" s="99"/>
-      <c r="U12" s="97"/>
-      <c r="V12" s="98"/>
-      <c r="W12" s="98"/>
-      <c r="X12" s="98"/>
-      <c r="Y12" s="98"/>
-      <c r="Z12" s="98"/>
-      <c r="AA12" s="98"/>
-      <c r="AB12" s="98"/>
-      <c r="AC12" s="98"/>
-      <c r="AD12" s="98"/>
-      <c r="AE12" s="98"/>
-      <c r="AF12" s="98"/>
-      <c r="AG12" s="98"/>
-      <c r="AH12" s="98"/>
-      <c r="AI12" s="98"/>
-      <c r="AJ12" s="98"/>
-      <c r="AK12" s="98"/>
-      <c r="AL12" s="99"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="135"/>
+      <c r="O12" s="135"/>
+      <c r="P12" s="135"/>
+      <c r="Q12" s="135"/>
+      <c r="R12" s="135"/>
+      <c r="S12" s="135"/>
+      <c r="T12" s="136"/>
+      <c r="U12" s="134"/>
+      <c r="V12" s="135"/>
+      <c r="W12" s="135"/>
+      <c r="X12" s="135"/>
+      <c r="Y12" s="135"/>
+      <c r="Z12" s="135"/>
+      <c r="AA12" s="135"/>
+      <c r="AB12" s="135"/>
+      <c r="AC12" s="135"/>
+      <c r="AD12" s="135"/>
+      <c r="AE12" s="135"/>
+      <c r="AF12" s="135"/>
+      <c r="AG12" s="135"/>
+      <c r="AH12" s="135"/>
+      <c r="AI12" s="135"/>
+      <c r="AJ12" s="135"/>
+      <c r="AK12" s="135"/>
+      <c r="AL12" s="136"/>
       <c r="AM12" s="8"/>
     </row>
-    <row r="13" spans="2:39" ht="11.1" customHeight="1">
+    <row r="13" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" s="20">
         <v>57</v>
@@ -2840,66 +2975,72 @@
       </c>
       <c r="AM13" s="8"/>
     </row>
-    <row r="14" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
-      <c r="P14" s="101"/>
-      <c r="Q14" s="101"/>
-      <c r="R14" s="101"/>
-      <c r="S14" s="101"/>
-      <c r="T14" s="102"/>
-      <c r="U14" s="97"/>
-      <c r="V14" s="98"/>
-      <c r="W14" s="98"/>
-      <c r="X14" s="98"/>
-      <c r="Y14" s="98"/>
-      <c r="Z14" s="98"/>
-      <c r="AA14" s="98"/>
-      <c r="AB14" s="98"/>
-      <c r="AC14" s="99"/>
-      <c r="AD14" s="97"/>
-      <c r="AE14" s="98"/>
-      <c r="AF14" s="98"/>
-      <c r="AG14" s="98"/>
-      <c r="AH14" s="98"/>
-      <c r="AI14" s="98"/>
-      <c r="AJ14" s="98"/>
-      <c r="AK14" s="98"/>
-      <c r="AL14" s="99"/>
+      <c r="C14" s="140" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="99"/>
+      <c r="Q14" s="99"/>
+      <c r="R14" s="99"/>
+      <c r="S14" s="99"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="145">
+        <v>43076</v>
+      </c>
+      <c r="V14" s="96"/>
+      <c r="W14" s="96"/>
+      <c r="X14" s="96"/>
+      <c r="Y14" s="96"/>
+      <c r="Z14" s="96"/>
+      <c r="AA14" s="96"/>
+      <c r="AB14" s="96"/>
+      <c r="AC14" s="97"/>
+      <c r="AD14" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE14" s="96"/>
+      <c r="AF14" s="96"/>
+      <c r="AG14" s="96"/>
+      <c r="AH14" s="96"/>
+      <c r="AI14" s="96"/>
+      <c r="AJ14" s="96"/>
+      <c r="AK14" s="96"/>
+      <c r="AL14" s="97"/>
       <c r="AM14" s="8"/>
     </row>
-    <row r="15" spans="2:39" ht="11.1" customHeight="1">
+    <row r="15" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="101"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="101"/>
-      <c r="N15" s="101"/>
-      <c r="O15" s="101"/>
-      <c r="P15" s="101"/>
-      <c r="Q15" s="101"/>
-      <c r="R15" s="101"/>
-      <c r="S15" s="101"/>
-      <c r="T15" s="102"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
+      <c r="P15" s="99"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="100"/>
       <c r="U15" s="22">
         <v>37</v>
       </c>
@@ -2932,47 +3073,51 @@
       </c>
       <c r="AM15" s="8"/>
     </row>
-    <row r="16" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="98"/>
-      <c r="P16" s="98"/>
-      <c r="Q16" s="98"/>
-      <c r="R16" s="98"/>
-      <c r="S16" s="98"/>
-      <c r="T16" s="99"/>
-      <c r="U16" s="97"/>
-      <c r="V16" s="98"/>
-      <c r="W16" s="98"/>
-      <c r="X16" s="98"/>
-      <c r="Y16" s="98"/>
-      <c r="Z16" s="98"/>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98"/>
-      <c r="AC16" s="99"/>
-      <c r="AD16" s="97"/>
-      <c r="AE16" s="98"/>
-      <c r="AF16" s="98"/>
-      <c r="AG16" s="98"/>
-      <c r="AH16" s="98"/>
-      <c r="AI16" s="98"/>
-      <c r="AJ16" s="98"/>
-      <c r="AK16" s="98"/>
-      <c r="AL16" s="99"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="97"/>
+      <c r="U16" s="95" t="s">
+        <v>168</v>
+      </c>
+      <c r="V16" s="96"/>
+      <c r="W16" s="96"/>
+      <c r="X16" s="96"/>
+      <c r="Y16" s="96"/>
+      <c r="Z16" s="96"/>
+      <c r="AA16" s="96"/>
+      <c r="AB16" s="96"/>
+      <c r="AC16" s="97"/>
+      <c r="AD16" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE16" s="96"/>
+      <c r="AF16" s="96"/>
+      <c r="AG16" s="96"/>
+      <c r="AH16" s="96"/>
+      <c r="AI16" s="96"/>
+      <c r="AJ16" s="96"/>
+      <c r="AK16" s="96"/>
+      <c r="AL16" s="97"/>
       <c r="AM16" s="8"/>
     </row>
-    <row r="17" spans="2:39" ht="11.1" customHeight="1">
+    <row r="17" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="25">
         <v>67</v>
@@ -3024,47 +3169,51 @@
       </c>
       <c r="AM17" s="8"/>
     </row>
-    <row r="18" spans="2:39" ht="74.25" customHeight="1">
+    <row r="18" spans="2:39" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="98"/>
-      <c r="P18" s="98"/>
-      <c r="Q18" s="98"/>
-      <c r="R18" s="98"/>
-      <c r="S18" s="98"/>
-      <c r="T18" s="99"/>
-      <c r="U18" s="97"/>
-      <c r="V18" s="98"/>
-      <c r="W18" s="98"/>
-      <c r="X18" s="98"/>
-      <c r="Y18" s="98"/>
-      <c r="Z18" s="98"/>
-      <c r="AA18" s="98"/>
-      <c r="AB18" s="98"/>
-      <c r="AC18" s="98"/>
-      <c r="AD18" s="98"/>
-      <c r="AE18" s="98"/>
-      <c r="AF18" s="98"/>
-      <c r="AG18" s="98"/>
-      <c r="AH18" s="98"/>
-      <c r="AI18" s="98"/>
-      <c r="AJ18" s="98"/>
-      <c r="AK18" s="98"/>
-      <c r="AL18" s="99"/>
+      <c r="C18" s="146" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="147"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="147"/>
+      <c r="K18" s="147"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="147"/>
+      <c r="P18" s="147"/>
+      <c r="Q18" s="147"/>
+      <c r="R18" s="147"/>
+      <c r="S18" s="147"/>
+      <c r="T18" s="148"/>
+      <c r="U18" s="149" t="s">
+        <v>172</v>
+      </c>
+      <c r="V18" s="150"/>
+      <c r="W18" s="150"/>
+      <c r="X18" s="150"/>
+      <c r="Y18" s="150"/>
+      <c r="Z18" s="150"/>
+      <c r="AA18" s="150"/>
+      <c r="AB18" s="150"/>
+      <c r="AC18" s="150"/>
+      <c r="AD18" s="150"/>
+      <c r="AE18" s="150"/>
+      <c r="AF18" s="150"/>
+      <c r="AG18" s="150"/>
+      <c r="AH18" s="150"/>
+      <c r="AI18" s="150"/>
+      <c r="AJ18" s="150"/>
+      <c r="AK18" s="150"/>
+      <c r="AL18" s="151"/>
       <c r="AM18" s="8"/>
     </row>
-    <row r="19" spans="2:39" ht="11.1" customHeight="1">
+    <row r="19" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" s="20">
         <v>39</v>
@@ -3128,47 +3277,49 @@
       </c>
       <c r="AM19" s="8"/>
     </row>
-    <row r="20" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="98"/>
-      <c r="N20" s="98"/>
-      <c r="O20" s="98"/>
-      <c r="P20" s="98"/>
-      <c r="Q20" s="98"/>
-      <c r="R20" s="98"/>
-      <c r="S20" s="98"/>
-      <c r="T20" s="99"/>
-      <c r="U20" s="97"/>
-      <c r="V20" s="98"/>
-      <c r="W20" s="98"/>
-      <c r="X20" s="98"/>
-      <c r="Y20" s="98"/>
-      <c r="Z20" s="98"/>
-      <c r="AA20" s="98"/>
-      <c r="AB20" s="98"/>
-      <c r="AC20" s="99"/>
-      <c r="AD20" s="97"/>
-      <c r="AE20" s="98"/>
-      <c r="AF20" s="98"/>
-      <c r="AG20" s="98"/>
-      <c r="AH20" s="98"/>
-      <c r="AI20" s="98"/>
-      <c r="AJ20" s="98"/>
-      <c r="AK20" s="98"/>
-      <c r="AL20" s="99"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="96"/>
+      <c r="R20" s="96"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="97"/>
+      <c r="U20" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="V20" s="96"/>
+      <c r="W20" s="96"/>
+      <c r="X20" s="96"/>
+      <c r="Y20" s="96"/>
+      <c r="Z20" s="96"/>
+      <c r="AA20" s="96"/>
+      <c r="AB20" s="96"/>
+      <c r="AC20" s="97"/>
+      <c r="AD20" s="95"/>
+      <c r="AE20" s="96"/>
+      <c r="AF20" s="96"/>
+      <c r="AG20" s="96"/>
+      <c r="AH20" s="96"/>
+      <c r="AI20" s="96"/>
+      <c r="AJ20" s="96"/>
+      <c r="AK20" s="96"/>
+      <c r="AL20" s="97"/>
       <c r="AM20" s="9"/>
     </row>
-    <row r="21" spans="2:39" ht="11.1" customHeight="1">
+    <row r="21" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="9"/>
       <c r="C21" s="20">
         <v>26</v>
@@ -3220,68 +3371,68 @@
       </c>
       <c r="AM21" s="9"/>
     </row>
-    <row r="22" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="101"/>
-      <c r="M22" s="101"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="101"/>
-      <c r="P22" s="101"/>
-      <c r="Q22" s="101"/>
-      <c r="R22" s="101"/>
-      <c r="S22" s="101"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="101"/>
-      <c r="V22" s="102"/>
-      <c r="W22" s="97"/>
-      <c r="X22" s="98"/>
-      <c r="Y22" s="98"/>
-      <c r="Z22" s="98"/>
-      <c r="AA22" s="98"/>
-      <c r="AB22" s="98"/>
-      <c r="AC22" s="98"/>
-      <c r="AD22" s="98"/>
-      <c r="AE22" s="98"/>
-      <c r="AF22" s="98"/>
-      <c r="AG22" s="98"/>
-      <c r="AH22" s="98"/>
-      <c r="AI22" s="98"/>
-      <c r="AJ22" s="98"/>
-      <c r="AK22" s="98"/>
-      <c r="AL22" s="99"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="99"/>
+      <c r="M22" s="99"/>
+      <c r="N22" s="99"/>
+      <c r="O22" s="99"/>
+      <c r="P22" s="99"/>
+      <c r="Q22" s="99"/>
+      <c r="R22" s="99"/>
+      <c r="S22" s="99"/>
+      <c r="T22" s="99"/>
+      <c r="U22" s="99"/>
+      <c r="V22" s="100"/>
+      <c r="W22" s="95"/>
+      <c r="X22" s="96"/>
+      <c r="Y22" s="96"/>
+      <c r="Z22" s="96"/>
+      <c r="AA22" s="96"/>
+      <c r="AB22" s="96"/>
+      <c r="AC22" s="96"/>
+      <c r="AD22" s="96"/>
+      <c r="AE22" s="96"/>
+      <c r="AF22" s="96"/>
+      <c r="AG22" s="96"/>
+      <c r="AH22" s="96"/>
+      <c r="AI22" s="96"/>
+      <c r="AJ22" s="96"/>
+      <c r="AK22" s="96"/>
+      <c r="AL22" s="97"/>
       <c r="AM22" s="9"/>
     </row>
-    <row r="23" spans="2:39" ht="11.1" customHeight="1">
+    <row r="23" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="101"/>
-      <c r="L23" s="101"/>
-      <c r="M23" s="101"/>
-      <c r="N23" s="101"/>
-      <c r="O23" s="101"/>
-      <c r="P23" s="101"/>
-      <c r="Q23" s="101"/>
-      <c r="R23" s="101"/>
-      <c r="S23" s="101"/>
-      <c r="T23" s="101"/>
-      <c r="U23" s="101"/>
-      <c r="V23" s="102"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="99"/>
+      <c r="L23" s="99"/>
+      <c r="M23" s="99"/>
+      <c r="N23" s="99"/>
+      <c r="O23" s="99"/>
+      <c r="P23" s="99"/>
+      <c r="Q23" s="99"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
+      <c r="U23" s="99"/>
+      <c r="V23" s="100"/>
       <c r="W23" s="22">
         <v>7</v>
       </c>
@@ -3306,47 +3457,49 @@
       </c>
       <c r="AM23" s="9"/>
     </row>
-    <row r="24" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="98"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="98"/>
-      <c r="N24" s="98"/>
-      <c r="O24" s="98"/>
-      <c r="P24" s="98"/>
-      <c r="Q24" s="98"/>
-      <c r="R24" s="98"/>
-      <c r="S24" s="98"/>
-      <c r="T24" s="98"/>
-      <c r="U24" s="98"/>
-      <c r="V24" s="99"/>
-      <c r="W24" s="97"/>
-      <c r="X24" s="98"/>
-      <c r="Y24" s="98"/>
-      <c r="Z24" s="98"/>
-      <c r="AA24" s="98"/>
-      <c r="AB24" s="98"/>
-      <c r="AC24" s="98"/>
-      <c r="AD24" s="98"/>
-      <c r="AE24" s="98"/>
-      <c r="AF24" s="98"/>
-      <c r="AG24" s="98"/>
-      <c r="AH24" s="98"/>
-      <c r="AI24" s="98"/>
-      <c r="AJ24" s="98"/>
-      <c r="AK24" s="98"/>
-      <c r="AL24" s="99"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="96"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="96"/>
+      <c r="L24" s="96"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="96"/>
+      <c r="O24" s="96"/>
+      <c r="P24" s="96"/>
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="96"/>
+      <c r="U24" s="96"/>
+      <c r="V24" s="97"/>
+      <c r="W24" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="X24" s="96"/>
+      <c r="Y24" s="96"/>
+      <c r="Z24" s="96"/>
+      <c r="AA24" s="96"/>
+      <c r="AB24" s="96"/>
+      <c r="AC24" s="96"/>
+      <c r="AD24" s="96"/>
+      <c r="AE24" s="96"/>
+      <c r="AF24" s="96"/>
+      <c r="AG24" s="96"/>
+      <c r="AH24" s="96"/>
+      <c r="AI24" s="96"/>
+      <c r="AJ24" s="96"/>
+      <c r="AK24" s="96"/>
+      <c r="AL24" s="97"/>
       <c r="AM24" s="9"/>
     </row>
-    <row r="25" spans="2:39" ht="12.95" customHeight="1">
+    <row r="25" spans="2:39" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -3386,7 +3539,7 @@
       <c r="AL25" s="14"/>
       <c r="AM25" s="9"/>
     </row>
-    <row r="26" spans="2:39" ht="11.1" customHeight="1">
+    <row r="26" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -3424,7 +3577,7 @@
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
     </row>
-    <row r="27" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -3466,7 +3619,7 @@
       <c r="AL27" s="10"/>
       <c r="AM27" s="9"/>
     </row>
-    <row r="28" spans="2:39" ht="9.9499999999999993" customHeight="1">
+    <row r="28" spans="2:39" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="25">
         <v>68</v>
@@ -3524,47 +3677,49 @@
       </c>
       <c r="AM28" s="9"/>
     </row>
-    <row r="29" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="104"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="104"/>
-      <c r="J29" s="104"/>
-      <c r="K29" s="104"/>
-      <c r="L29" s="104"/>
-      <c r="M29" s="104"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
-      <c r="T29" s="104"/>
-      <c r="U29" s="104"/>
-      <c r="V29" s="104"/>
-      <c r="W29" s="104"/>
-      <c r="X29" s="104"/>
-      <c r="Y29" s="104"/>
-      <c r="Z29" s="105"/>
-      <c r="AA29" s="103"/>
-      <c r="AB29" s="104"/>
-      <c r="AC29" s="104"/>
-      <c r="AD29" s="104"/>
-      <c r="AE29" s="104"/>
-      <c r="AF29" s="104"/>
-      <c r="AG29" s="104"/>
-      <c r="AH29" s="104"/>
-      <c r="AI29" s="104"/>
-      <c r="AJ29" s="104"/>
-      <c r="AK29" s="104"/>
-      <c r="AL29" s="105"/>
+      <c r="C29" s="101" t="s">
+        <v>176</v>
+      </c>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="102"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="102"/>
+      <c r="T29" s="102"/>
+      <c r="U29" s="102"/>
+      <c r="V29" s="102"/>
+      <c r="W29" s="102"/>
+      <c r="X29" s="102"/>
+      <c r="Y29" s="102"/>
+      <c r="Z29" s="103"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="102"/>
+      <c r="AC29" s="102"/>
+      <c r="AD29" s="102"/>
+      <c r="AE29" s="102"/>
+      <c r="AF29" s="102"/>
+      <c r="AG29" s="102"/>
+      <c r="AH29" s="102"/>
+      <c r="AI29" s="102"/>
+      <c r="AJ29" s="102"/>
+      <c r="AK29" s="102"/>
+      <c r="AL29" s="103"/>
       <c r="AM29" s="9"/>
     </row>
-    <row r="30" spans="2:39" ht="12.95" customHeight="1">
+    <row r="30" spans="2:39" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
@@ -3604,7 +3759,7 @@
       <c r="AL30" s="11"/>
       <c r="AM30" s="11"/>
     </row>
-    <row r="31" spans="2:39" ht="11.1" customHeight="1">
+    <row r="31" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -3642,7 +3797,7 @@
       <c r="AK31" s="6"/>
       <c r="AL31" s="6"/>
     </row>
-    <row r="32" spans="2:39" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:39" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -3684,7 +3839,7 @@
       <c r="AL32" s="10"/>
       <c r="AM32" s="9"/>
     </row>
-    <row r="33" spans="2:39" ht="11.1" customHeight="1">
+    <row r="33" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="25">
         <v>133</v>
@@ -3736,47 +3891,47 @@
       </c>
       <c r="AM33" s="9"/>
     </row>
-    <row r="34" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
-      <c r="C34" s="97"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="98"/>
-      <c r="M34" s="98"/>
-      <c r="N34" s="98"/>
-      <c r="O34" s="98"/>
-      <c r="P34" s="98"/>
-      <c r="Q34" s="98"/>
-      <c r="R34" s="98"/>
-      <c r="S34" s="98"/>
-      <c r="T34" s="99"/>
-      <c r="U34" s="97"/>
-      <c r="V34" s="98"/>
-      <c r="W34" s="98"/>
-      <c r="X34" s="98"/>
-      <c r="Y34" s="98"/>
-      <c r="Z34" s="98"/>
-      <c r="AA34" s="98"/>
-      <c r="AB34" s="98"/>
-      <c r="AC34" s="98"/>
-      <c r="AD34" s="98"/>
-      <c r="AE34" s="98"/>
-      <c r="AF34" s="98"/>
-      <c r="AG34" s="98"/>
-      <c r="AH34" s="98"/>
-      <c r="AI34" s="98"/>
-      <c r="AJ34" s="98"/>
-      <c r="AK34" s="98"/>
-      <c r="AL34" s="99"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="96"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="95"/>
+      <c r="V34" s="96"/>
+      <c r="W34" s="96"/>
+      <c r="X34" s="96"/>
+      <c r="Y34" s="96"/>
+      <c r="Z34" s="96"/>
+      <c r="AA34" s="96"/>
+      <c r="AB34" s="96"/>
+      <c r="AC34" s="96"/>
+      <c r="AD34" s="96"/>
+      <c r="AE34" s="96"/>
+      <c r="AF34" s="96"/>
+      <c r="AG34" s="96"/>
+      <c r="AH34" s="96"/>
+      <c r="AI34" s="96"/>
+      <c r="AJ34" s="96"/>
+      <c r="AK34" s="96"/>
+      <c r="AL34" s="97"/>
       <c r="AM34" s="9"/>
     </row>
-    <row r="35" spans="2:39" ht="12" customHeight="1">
+    <row r="35" spans="2:39" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="20">
         <v>132</v>
@@ -3828,47 +3983,47 @@
       </c>
       <c r="AM35" s="9"/>
     </row>
-    <row r="36" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
-      <c r="M36" s="98"/>
-      <c r="N36" s="98"/>
-      <c r="O36" s="98"/>
-      <c r="P36" s="98"/>
-      <c r="Q36" s="98"/>
-      <c r="R36" s="98"/>
-      <c r="S36" s="98"/>
-      <c r="T36" s="99"/>
-      <c r="U36" s="97"/>
-      <c r="V36" s="98"/>
-      <c r="W36" s="98"/>
-      <c r="X36" s="98"/>
-      <c r="Y36" s="98"/>
-      <c r="Z36" s="98"/>
-      <c r="AA36" s="98"/>
-      <c r="AB36" s="98"/>
-      <c r="AC36" s="98"/>
-      <c r="AD36" s="98"/>
-      <c r="AE36" s="98"/>
-      <c r="AF36" s="98"/>
-      <c r="AG36" s="98"/>
-      <c r="AH36" s="98"/>
-      <c r="AI36" s="98"/>
-      <c r="AJ36" s="98"/>
-      <c r="AK36" s="98"/>
-      <c r="AL36" s="99"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="96"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
+      <c r="Q36" s="96"/>
+      <c r="R36" s="96"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="95"/>
+      <c r="V36" s="96"/>
+      <c r="W36" s="96"/>
+      <c r="X36" s="96"/>
+      <c r="Y36" s="96"/>
+      <c r="Z36" s="96"/>
+      <c r="AA36" s="96"/>
+      <c r="AB36" s="96"/>
+      <c r="AC36" s="96"/>
+      <c r="AD36" s="96"/>
+      <c r="AE36" s="96"/>
+      <c r="AF36" s="96"/>
+      <c r="AG36" s="96"/>
+      <c r="AH36" s="96"/>
+      <c r="AI36" s="96"/>
+      <c r="AJ36" s="96"/>
+      <c r="AK36" s="96"/>
+      <c r="AL36" s="97"/>
       <c r="AM36" s="9"/>
     </row>
-    <row r="37" spans="2:39" ht="9.9499999999999993" customHeight="1">
+    <row r="37" spans="2:39" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="9"/>
       <c r="C37" s="20">
         <v>123</v>
@@ -3926,47 +4081,47 @@
       </c>
       <c r="AM37" s="9"/>
     </row>
-    <row r="38" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="97"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="98"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="98"/>
-      <c r="O38" s="98"/>
-      <c r="P38" s="98"/>
-      <c r="Q38" s="98"/>
-      <c r="R38" s="98"/>
-      <c r="S38" s="98"/>
-      <c r="T38" s="98"/>
-      <c r="U38" s="98"/>
-      <c r="V38" s="99"/>
-      <c r="W38" s="97"/>
-      <c r="X38" s="98"/>
-      <c r="Y38" s="98"/>
-      <c r="Z38" s="98"/>
-      <c r="AA38" s="98"/>
-      <c r="AB38" s="98"/>
-      <c r="AC38" s="98"/>
-      <c r="AD38" s="98"/>
-      <c r="AE38" s="98"/>
-      <c r="AF38" s="98"/>
-      <c r="AG38" s="98"/>
-      <c r="AH38" s="98"/>
-      <c r="AI38" s="98"/>
-      <c r="AJ38" s="98"/>
-      <c r="AK38" s="98"/>
-      <c r="AL38" s="99"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="96"/>
+      <c r="L38" s="96"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="96"/>
+      <c r="O38" s="96"/>
+      <c r="P38" s="96"/>
+      <c r="Q38" s="96"/>
+      <c r="R38" s="96"/>
+      <c r="S38" s="96"/>
+      <c r="T38" s="96"/>
+      <c r="U38" s="96"/>
+      <c r="V38" s="97"/>
+      <c r="W38" s="95"/>
+      <c r="X38" s="96"/>
+      <c r="Y38" s="96"/>
+      <c r="Z38" s="96"/>
+      <c r="AA38" s="96"/>
+      <c r="AB38" s="96"/>
+      <c r="AC38" s="96"/>
+      <c r="AD38" s="96"/>
+      <c r="AE38" s="96"/>
+      <c r="AF38" s="96"/>
+      <c r="AG38" s="96"/>
+      <c r="AH38" s="96"/>
+      <c r="AI38" s="96"/>
+      <c r="AJ38" s="96"/>
+      <c r="AK38" s="96"/>
+      <c r="AL38" s="97"/>
       <c r="AM38" s="9"/>
     </row>
-    <row r="39" spans="2:39" ht="14.1" customHeight="1">
+    <row r="39" spans="2:39" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -4006,7 +4161,7 @@
       <c r="AL39" s="9"/>
       <c r="AM39" s="9"/>
     </row>
-    <row r="40" spans="2:39" ht="11.1" customHeight="1">
+    <row r="40" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -4044,7 +4199,7 @@
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
     </row>
-    <row r="41" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -4086,7 +4241,7 @@
       <c r="AL41" s="9"/>
       <c r="AM41" s="9"/>
     </row>
-    <row r="42" spans="2:39" ht="9.9499999999999993" customHeight="1">
+    <row r="42" spans="2:39" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="9"/>
       <c r="C42" s="20">
         <v>128</v>
@@ -4132,47 +4287,47 @@
       </c>
       <c r="AM42" s="9"/>
     </row>
-    <row r="43" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="9"/>
-      <c r="C43" s="97"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
-      <c r="Q43" s="98"/>
-      <c r="R43" s="98"/>
-      <c r="S43" s="98"/>
-      <c r="T43" s="98"/>
-      <c r="U43" s="98"/>
-      <c r="V43" s="98"/>
-      <c r="W43" s="98"/>
-      <c r="X43" s="98"/>
-      <c r="Y43" s="98"/>
-      <c r="Z43" s="98"/>
-      <c r="AA43" s="98"/>
-      <c r="AB43" s="98"/>
-      <c r="AC43" s="98"/>
-      <c r="AD43" s="98"/>
-      <c r="AE43" s="98"/>
-      <c r="AF43" s="98"/>
-      <c r="AG43" s="98"/>
-      <c r="AH43" s="98"/>
-      <c r="AI43" s="98"/>
-      <c r="AJ43" s="98"/>
-      <c r="AK43" s="98"/>
-      <c r="AL43" s="99"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="96"/>
+      <c r="H43" s="96"/>
+      <c r="I43" s="96"/>
+      <c r="J43" s="96"/>
+      <c r="K43" s="96"/>
+      <c r="L43" s="96"/>
+      <c r="M43" s="96"/>
+      <c r="N43" s="96"/>
+      <c r="O43" s="96"/>
+      <c r="P43" s="96"/>
+      <c r="Q43" s="96"/>
+      <c r="R43" s="96"/>
+      <c r="S43" s="96"/>
+      <c r="T43" s="96"/>
+      <c r="U43" s="96"/>
+      <c r="V43" s="96"/>
+      <c r="W43" s="96"/>
+      <c r="X43" s="96"/>
+      <c r="Y43" s="96"/>
+      <c r="Z43" s="96"/>
+      <c r="AA43" s="96"/>
+      <c r="AB43" s="96"/>
+      <c r="AC43" s="96"/>
+      <c r="AD43" s="96"/>
+      <c r="AE43" s="96"/>
+      <c r="AF43" s="96"/>
+      <c r="AG43" s="96"/>
+      <c r="AH43" s="96"/>
+      <c r="AI43" s="96"/>
+      <c r="AJ43" s="96"/>
+      <c r="AK43" s="96"/>
+      <c r="AL43" s="97"/>
       <c r="AM43" s="9"/>
     </row>
-    <row r="44" spans="2:39" ht="11.1" customHeight="1">
+    <row r="44" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="9"/>
       <c r="C44" s="20">
         <v>129</v>
@@ -4218,47 +4373,47 @@
       </c>
       <c r="AM44" s="9"/>
     </row>
-    <row r="45" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="9"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="98"/>
-      <c r="E45" s="98"/>
-      <c r="F45" s="98"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="98"/>
-      <c r="I45" s="98"/>
-      <c r="J45" s="98"/>
-      <c r="K45" s="98"/>
-      <c r="L45" s="98"/>
-      <c r="M45" s="98"/>
-      <c r="N45" s="98"/>
-      <c r="O45" s="98"/>
-      <c r="P45" s="98"/>
-      <c r="Q45" s="98"/>
-      <c r="R45" s="98"/>
-      <c r="S45" s="98"/>
-      <c r="T45" s="98"/>
-      <c r="U45" s="98"/>
-      <c r="V45" s="98"/>
-      <c r="W45" s="98"/>
-      <c r="X45" s="98"/>
-      <c r="Y45" s="98"/>
-      <c r="Z45" s="98"/>
-      <c r="AA45" s="98"/>
-      <c r="AB45" s="98"/>
-      <c r="AC45" s="98"/>
-      <c r="AD45" s="98"/>
-      <c r="AE45" s="98"/>
-      <c r="AF45" s="98"/>
-      <c r="AG45" s="98"/>
-      <c r="AH45" s="98"/>
-      <c r="AI45" s="98"/>
-      <c r="AJ45" s="98"/>
-      <c r="AK45" s="98"/>
-      <c r="AL45" s="99"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
+      <c r="H45" s="96"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
+      <c r="L45" s="96"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="96"/>
+      <c r="O45" s="96"/>
+      <c r="P45" s="96"/>
+      <c r="Q45" s="96"/>
+      <c r="R45" s="96"/>
+      <c r="S45" s="96"/>
+      <c r="T45" s="96"/>
+      <c r="U45" s="96"/>
+      <c r="V45" s="96"/>
+      <c r="W45" s="96"/>
+      <c r="X45" s="96"/>
+      <c r="Y45" s="96"/>
+      <c r="Z45" s="96"/>
+      <c r="AA45" s="96"/>
+      <c r="AB45" s="96"/>
+      <c r="AC45" s="96"/>
+      <c r="AD45" s="96"/>
+      <c r="AE45" s="96"/>
+      <c r="AF45" s="96"/>
+      <c r="AG45" s="96"/>
+      <c r="AH45" s="96"/>
+      <c r="AI45" s="96"/>
+      <c r="AJ45" s="96"/>
+      <c r="AK45" s="96"/>
+      <c r="AL45" s="97"/>
       <c r="AM45" s="9"/>
     </row>
-    <row r="46" spans="2:39" ht="11.1" customHeight="1">
+    <row r="46" spans="2:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="20">
         <v>131</v>
@@ -4310,47 +4465,47 @@
       </c>
       <c r="AM46" s="9"/>
     </row>
-    <row r="47" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
-      <c r="C47" s="97"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="98"/>
-      <c r="I47" s="98"/>
-      <c r="J47" s="98"/>
-      <c r="K47" s="98"/>
-      <c r="L47" s="98"/>
-      <c r="M47" s="98"/>
-      <c r="N47" s="98"/>
-      <c r="O47" s="98"/>
-      <c r="P47" s="98"/>
-      <c r="Q47" s="98"/>
-      <c r="R47" s="98"/>
-      <c r="S47" s="98"/>
-      <c r="T47" s="99"/>
-      <c r="U47" s="97"/>
-      <c r="V47" s="98"/>
-      <c r="W47" s="98"/>
-      <c r="X47" s="98"/>
-      <c r="Y47" s="98"/>
-      <c r="Z47" s="98"/>
-      <c r="AA47" s="98"/>
-      <c r="AB47" s="98"/>
-      <c r="AC47" s="98"/>
-      <c r="AD47" s="98"/>
-      <c r="AE47" s="98"/>
-      <c r="AF47" s="98"/>
-      <c r="AG47" s="98"/>
-      <c r="AH47" s="98"/>
-      <c r="AI47" s="98"/>
-      <c r="AJ47" s="98"/>
-      <c r="AK47" s="98"/>
-      <c r="AL47" s="99"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="96"/>
+      <c r="J47" s="96"/>
+      <c r="K47" s="96"/>
+      <c r="L47" s="96"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="96"/>
+      <c r="O47" s="96"/>
+      <c r="P47" s="96"/>
+      <c r="Q47" s="96"/>
+      <c r="R47" s="96"/>
+      <c r="S47" s="96"/>
+      <c r="T47" s="97"/>
+      <c r="U47" s="95"/>
+      <c r="V47" s="96"/>
+      <c r="W47" s="96"/>
+      <c r="X47" s="96"/>
+      <c r="Y47" s="96"/>
+      <c r="Z47" s="96"/>
+      <c r="AA47" s="96"/>
+      <c r="AB47" s="96"/>
+      <c r="AC47" s="96"/>
+      <c r="AD47" s="96"/>
+      <c r="AE47" s="96"/>
+      <c r="AF47" s="96"/>
+      <c r="AG47" s="96"/>
+      <c r="AH47" s="96"/>
+      <c r="AI47" s="96"/>
+      <c r="AJ47" s="96"/>
+      <c r="AK47" s="96"/>
+      <c r="AL47" s="97"/>
       <c r="AM47" s="9"/>
     </row>
-    <row r="48" spans="2:39" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="2:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -4390,130 +4545,137 @@
       <c r="AL48" s="9"/>
       <c r="AM48" s="9"/>
     </row>
-    <row r="49" ht="20.100000000000001" customHeight="1"/>
-    <row r="50" ht="20.100000000000001" customHeight="1"/>
-    <row r="51" ht="20.100000000000001" customHeight="1"/>
-    <row r="52" ht="20.100000000000001" customHeight="1"/>
-    <row r="53" ht="20.100000000000001" customHeight="1"/>
-    <row r="54" ht="20.100000000000001" customHeight="1"/>
-    <row r="55" ht="20.100000000000001" customHeight="1"/>
-    <row r="56" ht="20.100000000000001" customHeight="1"/>
-    <row r="57" ht="20.100000000000001" customHeight="1"/>
-    <row r="58" ht="20.100000000000001" customHeight="1"/>
-    <row r="59" ht="20.100000000000001" customHeight="1"/>
-    <row r="60" ht="20.100000000000001" customHeight="1"/>
-    <row r="61" ht="20.100000000000001" customHeight="1"/>
-    <row r="62" ht="20.100000000000001" customHeight="1"/>
-    <row r="63" ht="20.100000000000001" customHeight="1"/>
-    <row r="64" ht="20.100000000000001" customHeight="1"/>
-    <row r="65" ht="20.100000000000001" customHeight="1"/>
-    <row r="66" ht="20.100000000000001" customHeight="1"/>
-    <row r="67" ht="20.100000000000001" customHeight="1"/>
-    <row r="68" ht="20.100000000000001" customHeight="1"/>
-    <row r="69" ht="20.100000000000001" customHeight="1"/>
-    <row r="70" ht="20.100000000000001" customHeight="1"/>
-    <row r="71" ht="20.100000000000001" customHeight="1"/>
-    <row r="72" ht="20.100000000000001" customHeight="1"/>
-    <row r="73" ht="20.100000000000001" customHeight="1"/>
-    <row r="74" ht="20.100000000000001" customHeight="1"/>
-    <row r="75" ht="20.100000000000001" customHeight="1"/>
-    <row r="76" ht="20.100000000000001" customHeight="1"/>
-    <row r="77" ht="20.100000000000001" customHeight="1"/>
-    <row r="78" ht="20.100000000000001" customHeight="1"/>
-    <row r="79" ht="20.100000000000001" customHeight="1"/>
-    <row r="80" ht="20.100000000000001" customHeight="1"/>
-    <row r="81" ht="20.100000000000001" customHeight="1"/>
-    <row r="82" ht="20.100000000000001" customHeight="1"/>
-    <row r="83" ht="20.100000000000001" customHeight="1"/>
-    <row r="84" ht="20.100000000000001" customHeight="1"/>
-    <row r="85" ht="20.100000000000001" customHeight="1"/>
-    <row r="86" ht="20.100000000000001" customHeight="1"/>
-    <row r="87" ht="20.100000000000001" customHeight="1"/>
-    <row r="88" ht="20.100000000000001" customHeight="1"/>
-    <row r="89" ht="20.100000000000001" customHeight="1"/>
-    <row r="90" ht="20.100000000000001" customHeight="1"/>
-    <row r="91" ht="20.100000000000001" customHeight="1"/>
-    <row r="92" ht="20.100000000000001" customHeight="1"/>
-    <row r="93" ht="20.100000000000001" customHeight="1"/>
-    <row r="94" ht="20.100000000000001" customHeight="1"/>
-    <row r="95" ht="20.100000000000001" customHeight="1"/>
-    <row r="96" ht="20.100000000000001" customHeight="1"/>
-    <row r="97" ht="20.100000000000001" customHeight="1"/>
-    <row r="98" ht="20.100000000000001" customHeight="1"/>
-    <row r="99" ht="20.100000000000001" customHeight="1"/>
-    <row r="100" ht="20.100000000000001" customHeight="1"/>
-    <row r="101" ht="20.100000000000001" customHeight="1"/>
-    <row r="102" ht="20.100000000000001" customHeight="1"/>
-    <row r="103" ht="20.100000000000001" customHeight="1"/>
-    <row r="104" ht="20.100000000000001" customHeight="1"/>
-    <row r="105" ht="20.100000000000001" customHeight="1"/>
-    <row r="106" ht="20.100000000000001" customHeight="1"/>
-    <row r="107" ht="20.100000000000001" customHeight="1"/>
-    <row r="108" ht="20.100000000000001" customHeight="1"/>
-    <row r="109" ht="20.100000000000001" customHeight="1"/>
-    <row r="110" ht="20.100000000000001" customHeight="1"/>
-    <row r="111" ht="20.100000000000001" customHeight="1"/>
-    <row r="112" ht="20.100000000000001" customHeight="1"/>
-    <row r="113" ht="20.100000000000001" customHeight="1"/>
-    <row r="114" ht="20.100000000000001" customHeight="1"/>
-    <row r="115" ht="20.100000000000001" customHeight="1"/>
-    <row r="116" ht="20.100000000000001" customHeight="1"/>
-    <row r="117" ht="20.100000000000001" customHeight="1"/>
-    <row r="118" ht="20.100000000000001" customHeight="1"/>
-    <row r="119" ht="20.100000000000001" customHeight="1"/>
-    <row r="120" ht="20.100000000000001" customHeight="1"/>
-    <row r="121" ht="20.100000000000001" customHeight="1"/>
-    <row r="122" ht="20.100000000000001" customHeight="1"/>
-    <row r="123" ht="20.100000000000001" customHeight="1"/>
-    <row r="124" ht="20.100000000000001" customHeight="1"/>
-    <row r="125" ht="20.100000000000001" customHeight="1"/>
-    <row r="126" ht="20.100000000000001" customHeight="1"/>
-    <row r="127" ht="20.100000000000001" customHeight="1"/>
-    <row r="128" ht="20.100000000000001" customHeight="1"/>
-    <row r="129" ht="20.100000000000001" customHeight="1"/>
-    <row r="130" ht="20.100000000000001" customHeight="1"/>
-    <row r="131" ht="20.100000000000001" customHeight="1"/>
-    <row r="132" ht="20.100000000000001" customHeight="1"/>
-    <row r="133" ht="20.100000000000001" customHeight="1"/>
-    <row r="134" ht="20.100000000000001" customHeight="1"/>
-    <row r="135" ht="20.100000000000001" customHeight="1"/>
-    <row r="136" ht="20.100000000000001" customHeight="1"/>
-    <row r="137" ht="20.100000000000001" customHeight="1"/>
-    <row r="138" ht="20.100000000000001" customHeight="1"/>
-    <row r="139" ht="20.100000000000001" customHeight="1"/>
-    <row r="140" ht="20.100000000000001" customHeight="1"/>
-    <row r="141" ht="20.100000000000001" customHeight="1"/>
-    <row r="142" ht="20.100000000000001" customHeight="1"/>
-    <row r="143" ht="20.100000000000001" customHeight="1"/>
-    <row r="144" ht="20.100000000000001" customHeight="1"/>
-    <row r="145" ht="20.100000000000001" customHeight="1"/>
-    <row r="146" ht="20.100000000000001" customHeight="1"/>
-    <row r="147" ht="20.100000000000001" customHeight="1"/>
-    <row r="148" ht="20.100000000000001" customHeight="1"/>
-    <row r="149" ht="20.100000000000001" customHeight="1"/>
-    <row r="150" ht="20.100000000000001" customHeight="1"/>
-    <row r="151" ht="20.100000000000001" customHeight="1"/>
-    <row r="152" ht="20.100000000000001" customHeight="1"/>
-    <row r="153" ht="20.100000000000001" customHeight="1"/>
-    <row r="154" ht="20.100000000000001" customHeight="1"/>
-    <row r="155" ht="20.100000000000001" customHeight="1"/>
-    <row r="156" ht="20.100000000000001" customHeight="1"/>
-    <row r="157" ht="20.100000000000001" customHeight="1"/>
-    <row r="158" ht="20.100000000000001" customHeight="1"/>
-    <row r="159" ht="20.100000000000001" customHeight="1"/>
-    <row r="160" ht="20.100000000000001" customHeight="1"/>
+    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tRZjg5iePoHIurj4DcCH3ORWMCG1kAap65T8XU6NpMuf2IIsU4bbQ97D36LadeVtXOBGEFwC1xCZKV3KdRwhQQ==" saltValue="sc4QtkjHNagNG0zxDyDa3w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="38">
-    <mergeCell ref="C43:AL43"/>
-    <mergeCell ref="C45:AL45"/>
-    <mergeCell ref="C47:T47"/>
-    <mergeCell ref="U47:AL47"/>
-    <mergeCell ref="U36:AL36"/>
-    <mergeCell ref="W38:AL38"/>
-    <mergeCell ref="G38:V38"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C36:T36"/>
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="AC3:AL3"/>
+    <mergeCell ref="AC2:AL2"/>
+    <mergeCell ref="L2:AB2"/>
+    <mergeCell ref="L3:AB3"/>
+    <mergeCell ref="C8:T8"/>
+    <mergeCell ref="U8:AL8"/>
+    <mergeCell ref="U10:AL12"/>
+    <mergeCell ref="C10:T12"/>
+    <mergeCell ref="C18:T18"/>
+    <mergeCell ref="U18:AL18"/>
+    <mergeCell ref="AD16:AL16"/>
+    <mergeCell ref="AD14:AL14"/>
+    <mergeCell ref="U14:AC14"/>
+    <mergeCell ref="U16:AC16"/>
     <mergeCell ref="C34:T34"/>
     <mergeCell ref="C14:T16"/>
     <mergeCell ref="W24:AL24"/>
@@ -4527,22 +4689,15 @@
     <mergeCell ref="C22:V24"/>
     <mergeCell ref="W22:AL22"/>
     <mergeCell ref="AD20:AL20"/>
-    <mergeCell ref="C8:T8"/>
-    <mergeCell ref="U8:AL8"/>
-    <mergeCell ref="U10:AL12"/>
-    <mergeCell ref="C10:T12"/>
-    <mergeCell ref="C18:T18"/>
-    <mergeCell ref="U18:AL18"/>
-    <mergeCell ref="AD16:AL16"/>
-    <mergeCell ref="AD14:AL14"/>
-    <mergeCell ref="U14:AC14"/>
-    <mergeCell ref="U16:AC16"/>
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="AC3:AL3"/>
-    <mergeCell ref="AC2:AL2"/>
-    <mergeCell ref="L2:AB2"/>
-    <mergeCell ref="L3:AB3"/>
+    <mergeCell ref="C43:AL43"/>
+    <mergeCell ref="C45:AL45"/>
+    <mergeCell ref="C47:T47"/>
+    <mergeCell ref="U47:AL47"/>
+    <mergeCell ref="U36:AL36"/>
+    <mergeCell ref="W38:AL38"/>
+    <mergeCell ref="G38:V38"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C36:T36"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
@@ -4581,7 +4736,8 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.98" header="0" footer="0.39370078740157483"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -4597,11 +4753,11 @@
   </sheetPr>
   <dimension ref="A1:BF90"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:J2"/>
+    <sheetView showRuler="0" topLeftCell="A7" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="4" customWidth="1"/>
@@ -4620,7 +4776,7 @@
     <col min="59" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="33.950000000000003" customHeight="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -4638,12 +4794,12 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="46.5" customHeight="1">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="129"/>
       <c r="C2" s="129"/>
       <c r="D2" s="91"/>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="104" t="s">
         <v>164</v>
       </c>
       <c r="F2" s="112"/>
@@ -4660,7 +4816,7 @@
       <c r="O2" s="112"/>
       <c r="P2" s="7"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="37.5" customHeight="1">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="128" t="s">
         <v>163</v>
@@ -4684,7 +4840,7 @@
       <c r="O3" s="112"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="26.1" customHeight="1" thickBot="1">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -4702,7 +4858,7 @@
       <c r="O4" s="24"/>
       <c r="P4" s="27"/>
     </row>
-    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="65"/>
       <c r="B5" s="113" t="s">
         <v>0</v>
@@ -4732,7 +4888,7 @@
       </c>
       <c r="P5" s="69"/>
     </row>
-    <row r="6" spans="1:16" ht="18.95" customHeight="1">
+    <row r="6" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65"/>
       <c r="B6" s="114"/>
       <c r="C6" s="117"/>
@@ -4752,7 +4908,7 @@
       <c r="O6" s="110"/>
       <c r="P6" s="69"/>
     </row>
-    <row r="7" spans="1:16" ht="48" customHeight="1" thickBot="1">
+    <row r="7" spans="1:16" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
       <c r="B7" s="115"/>
       <c r="C7" s="118"/>
@@ -4786,7 +4942,7 @@
       <c r="O7" s="111"/>
       <c r="P7" s="69"/>
     </row>
-    <row r="8" spans="1:16" ht="30.95" customHeight="1">
+    <row r="8" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="66"/>
       <c r="B8" s="43">
         <v>132</v>
@@ -4830,7 +4986,7 @@
       <c r="O8" s="57"/>
       <c r="P8" s="69"/>
     </row>
-    <row r="9" spans="1:16" ht="30.95" customHeight="1">
+    <row r="9" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66"/>
       <c r="B9" s="44">
         <v>9</v>
@@ -4876,7 +5032,7 @@
       </c>
       <c r="P9" s="69"/>
     </row>
-    <row r="10" spans="1:16" ht="30.95" customHeight="1">
+    <row r="10" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="66"/>
       <c r="B10" s="45">
         <v>134</v>
@@ -4920,7 +5076,7 @@
       <c r="O10" s="59"/>
       <c r="P10" s="69"/>
     </row>
-    <row r="11" spans="1:16" ht="30.95" customHeight="1">
+    <row r="11" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
       <c r="B11" s="44">
         <v>7</v>
@@ -4964,7 +5120,7 @@
       <c r="O11" s="59"/>
       <c r="P11" s="69"/>
     </row>
-    <row r="12" spans="1:16" ht="57.95" customHeight="1">
+    <row r="12" spans="1:16" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="66"/>
       <c r="B12" s="44">
         <v>1</v>
@@ -5010,7 +5166,7 @@
       </c>
       <c r="P12" s="69"/>
     </row>
-    <row r="13" spans="1:16" ht="30.95" customHeight="1">
+    <row r="13" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="66"/>
       <c r="B13" s="45">
         <v>135</v>
@@ -5054,7 +5210,7 @@
       <c r="O13" s="59"/>
       <c r="P13" s="69"/>
     </row>
-    <row r="14" spans="1:16" ht="191.1" customHeight="1">
+    <row r="14" spans="1:16" ht="191.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
       <c r="B14" s="46">
         <v>68</v>
@@ -5098,7 +5254,7 @@
       <c r="O14" s="59"/>
       <c r="P14" s="69"/>
     </row>
-    <row r="15" spans="1:16" ht="89.1" customHeight="1">
+    <row r="15" spans="1:16" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="66"/>
       <c r="B15" s="44">
         <v>53</v>
@@ -5142,7 +5298,7 @@
       <c r="O15" s="59"/>
       <c r="P15" s="69"/>
     </row>
-    <row r="16" spans="1:16" ht="42" customHeight="1">
+    <row r="16" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66"/>
       <c r="B16" s="44">
         <v>26</v>
@@ -5186,7 +5342,7 @@
       <c r="O16" s="59"/>
       <c r="P16" s="69"/>
     </row>
-    <row r="17" spans="1:16" ht="65.099999999999994" customHeight="1">
+    <row r="17" spans="1:16" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
       <c r="B17" s="47">
         <v>131</v>
@@ -5230,7 +5386,7 @@
       <c r="O17" s="59"/>
       <c r="P17" s="69"/>
     </row>
-    <row r="18" spans="1:16" ht="30.95" customHeight="1">
+    <row r="18" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="66"/>
       <c r="B18" s="45">
         <v>113</v>
@@ -5274,7 +5430,7 @@
       <c r="O18" s="59"/>
       <c r="P18" s="69"/>
     </row>
-    <row r="19" spans="1:16" ht="42" customHeight="1">
+    <row r="19" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="66"/>
       <c r="B19" s="44">
         <v>39</v>
@@ -5320,7 +5476,7 @@
       </c>
       <c r="P19" s="69"/>
     </row>
-    <row r="20" spans="1:16" ht="57" customHeight="1">
+    <row r="20" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="66"/>
       <c r="B20" s="44">
         <v>10</v>
@@ -5364,7 +5520,7 @@
       <c r="O20" s="59"/>
       <c r="P20" s="69"/>
     </row>
-    <row r="21" spans="1:16" ht="30.95" customHeight="1">
+    <row r="21" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="66"/>
       <c r="B21" s="45">
         <v>82</v>
@@ -5408,7 +5564,7 @@
       <c r="O21" s="59"/>
       <c r="P21" s="69"/>
     </row>
-    <row r="22" spans="1:16" ht="45" customHeight="1">
+    <row r="22" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="66"/>
       <c r="B22" s="44">
         <v>33</v>
@@ -5452,7 +5608,7 @@
       <c r="O22" s="59"/>
       <c r="P22" s="69"/>
     </row>
-    <row r="23" spans="1:16" ht="42" customHeight="1">
+    <row r="23" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="66"/>
       <c r="B23" s="44">
         <v>55</v>
@@ -5496,7 +5652,7 @@
       <c r="O23" s="59"/>
       <c r="P23" s="69"/>
     </row>
-    <row r="24" spans="1:16" ht="51.95" customHeight="1">
+    <row r="24" spans="1:16" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="66"/>
       <c r="B24" s="44">
         <v>17</v>
@@ -5538,7 +5694,7 @@
       <c r="O24" s="59"/>
       <c r="P24" s="69"/>
     </row>
-    <row r="25" spans="1:16" ht="30.95" customHeight="1">
+    <row r="25" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="66"/>
       <c r="B25" s="44">
         <v>37</v>
@@ -5582,7 +5738,7 @@
       <c r="O25" s="59"/>
       <c r="P25" s="69"/>
     </row>
-    <row r="26" spans="1:16" ht="30.95" customHeight="1">
+    <row r="26" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="66"/>
       <c r="B26" s="45">
         <v>136</v>
@@ -5626,7 +5782,7 @@
       <c r="O26" s="59"/>
       <c r="P26" s="69"/>
     </row>
-    <row r="27" spans="1:16" ht="69" customHeight="1">
+    <row r="27" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="66"/>
       <c r="B27" s="45">
         <v>130</v>
@@ -5670,7 +5826,7 @@
       <c r="O27" s="59"/>
       <c r="P27" s="69"/>
     </row>
-    <row r="28" spans="1:16" ht="107.1" customHeight="1">
+    <row r="28" spans="1:16" ht="107.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
       <c r="B28" s="45">
         <v>128</v>
@@ -5714,7 +5870,7 @@
       <c r="O28" s="59"/>
       <c r="P28" s="69"/>
     </row>
-    <row r="29" spans="1:16" ht="30.95" customHeight="1">
+    <row r="29" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="66"/>
       <c r="B29" s="45">
         <v>93</v>
@@ -5758,7 +5914,7 @@
       <c r="O29" s="59"/>
       <c r="P29" s="69"/>
     </row>
-    <row r="30" spans="1:16" ht="36.950000000000003" customHeight="1">
+    <row r="30" spans="1:16" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="66"/>
       <c r="B30" s="45">
         <v>97</v>
@@ -5802,7 +5958,7 @@
       <c r="O30" s="59"/>
       <c r="P30" s="69"/>
     </row>
-    <row r="31" spans="1:16" ht="39" customHeight="1">
+    <row r="31" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="66"/>
       <c r="B31" s="44">
         <v>40</v>
@@ -5848,7 +6004,7 @@
       </c>
       <c r="P31" s="69"/>
     </row>
-    <row r="32" spans="1:16" ht="36" customHeight="1">
+    <row r="32" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="66"/>
       <c r="B32" s="45">
         <v>67</v>
@@ -5892,7 +6048,7 @@
       <c r="O32" s="59"/>
       <c r="P32" s="69"/>
     </row>
-    <row r="33" spans="1:16" ht="30.95" customHeight="1">
+    <row r="33" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="66"/>
       <c r="B33" s="45">
         <v>133</v>
@@ -5936,7 +6092,7 @@
       <c r="O33" s="59"/>
       <c r="P33" s="69"/>
     </row>
-    <row r="34" spans="1:16" ht="30.95" customHeight="1">
+    <row r="34" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="66"/>
       <c r="B34" s="48">
         <v>31</v>
@@ -5980,7 +6136,7 @@
       <c r="O34" s="59"/>
       <c r="P34" s="69"/>
     </row>
-    <row r="35" spans="1:16" ht="30.95" customHeight="1">
+    <row r="35" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="66"/>
       <c r="B35" s="44">
         <v>57</v>
@@ -6026,7 +6182,7 @@
       </c>
       <c r="P35" s="69"/>
     </row>
-    <row r="36" spans="1:16" ht="63.95" customHeight="1">
+    <row r="36" spans="1:16" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="66"/>
       <c r="B36" s="44">
         <v>66</v>
@@ -6070,7 +6226,7 @@
       <c r="O36" s="59"/>
       <c r="P36" s="69"/>
     </row>
-    <row r="37" spans="1:16" ht="36" customHeight="1">
+    <row r="37" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="66"/>
       <c r="B37" s="44">
         <v>64</v>
@@ -6114,7 +6270,7 @@
       <c r="O37" s="59"/>
       <c r="P37" s="69"/>
     </row>
-    <row r="38" spans="1:16" ht="63.95" customHeight="1">
+    <row r="38" spans="1:16" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="66"/>
       <c r="B38" s="45">
         <v>129</v>
@@ -6158,7 +6314,7 @@
       <c r="O38" s="59"/>
       <c r="P38" s="69"/>
     </row>
-    <row r="39" spans="1:16" ht="30.95" customHeight="1">
+    <row r="39" spans="1:16" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="66"/>
       <c r="B39" s="45">
         <v>72</v>
@@ -6202,7 +6358,7 @@
       <c r="O39" s="59"/>
       <c r="P39" s="69"/>
     </row>
-    <row r="40" spans="1:16" ht="33.950000000000003" customHeight="1" thickBot="1">
+    <row r="40" spans="1:16" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="66"/>
       <c r="B40" s="49">
         <v>123</v>
@@ -6246,7 +6402,7 @@
       <c r="O40" s="60"/>
       <c r="P40" s="69"/>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="68"/>
       <c r="B41" s="69"/>
       <c r="C41" s="69"/>
@@ -6264,199 +6420,199 @@
       <c r="O41" s="69"/>
       <c r="P41" s="69"/>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1">
+    <row r="42" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1">
+    <row r="43" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1">
+    <row r="44" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1">
+    <row r="45" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1">
+    <row r="46" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1">
+    <row r="47" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1">
+    <row r="48" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="5:6" s="1" customFormat="1">
+    <row r="49" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="5:6" s="1" customFormat="1">
+    <row r="50" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="5:6" s="1" customFormat="1">
+    <row r="51" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="5:6" s="1" customFormat="1">
+    <row r="52" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="5:6" s="1" customFormat="1">
+    <row r="53" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="5:6" s="1" customFormat="1">
+    <row r="54" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="5:6" s="1" customFormat="1">
+    <row r="55" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="5:6" s="1" customFormat="1">
+    <row r="56" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="5:6" s="1" customFormat="1">
+    <row r="57" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="5:6" s="1" customFormat="1">
+    <row r="58" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="5:6" s="1" customFormat="1">
+    <row r="59" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="5:6" s="1" customFormat="1">
+    <row r="60" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="5:6" s="1" customFormat="1">
+    <row r="61" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="5:6" s="1" customFormat="1">
+    <row r="62" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="5:6" s="1" customFormat="1">
+    <row r="63" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="5:6" s="1" customFormat="1">
+    <row r="64" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="5:6" s="1" customFormat="1">
+    <row r="65" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="5:6" s="1" customFormat="1">
+    <row r="66" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="5:6" s="1" customFormat="1">
+    <row r="67" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="5:6" s="1" customFormat="1">
+    <row r="68" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="5:6" s="1" customFormat="1">
+    <row r="69" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="5:6" s="1" customFormat="1">
+    <row r="70" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="5:6" s="1" customFormat="1">
+    <row r="71" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="5:6" s="1" customFormat="1">
+    <row r="72" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="5:6" s="1" customFormat="1">
+    <row r="73" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="5:6" s="1" customFormat="1">
+    <row r="74" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="5:6" s="1" customFormat="1">
+    <row r="75" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="5:6" s="1" customFormat="1">
+    <row r="76" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="5:6" s="1" customFormat="1">
+    <row r="77" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="5:6" s="1" customFormat="1">
+    <row r="78" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="5:6" s="1" customFormat="1">
+    <row r="79" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="5:6" s="1" customFormat="1">
+    <row r="80" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="5:6" s="1" customFormat="1">
+    <row r="81" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="5:6" s="1" customFormat="1">
+    <row r="82" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="5:6" s="1" customFormat="1">
+    <row r="83" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="5:6" s="1" customFormat="1">
+    <row r="84" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="5:6" s="1" customFormat="1">
+    <row r="85" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="5:6" s="1" customFormat="1">
+    <row r="86" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="5:6" s="1" customFormat="1">
+    <row r="87" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="5:6" s="1" customFormat="1">
+    <row r="88" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="5:6" s="1" customFormat="1">
+    <row r="89" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="5:6" s="1" customFormat="1">
+    <row r="90" spans="5:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>

</xml_diff>